<commit_message>
use map(2) to automate read-in of .csvs
</commit_message>
<xml_diff>
--- a/INPUT-FILES/OES-INPUT-TABLES/TOD rating scale lookup outline.xlsx
+++ b/INPUT-FILES/OES-INPUT-TABLES/TOD rating scale lookup outline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wpspublish1-my.sharepoint.com/personal/aklein_wpspublish_com/Documents/Desktop/TOD/OES/input files for rating scales/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Library/CloudStorage/OneDrive-WesternPsychologicalServices/Desktop/R/TOD-R/INPUT-FILES/OES-INPUT-TABLES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EEB09F71-25B9-4C25-8656-1574AF12C292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4149409B-4614-0C4C-A4EC-72892F68122E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30690" yWindow="1095" windowWidth="12795" windowHeight="13575"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOD rating scale lookup" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>version</t>
   </si>
@@ -95,12 +95,18 @@
   </si>
   <si>
     <t>risk_level</t>
+  </si>
+  <si>
+    <t>Calculate actual intervals, based on these CVs</t>
+  </si>
+  <si>
+    <t>Collapse rater and norm_group into single col</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -584,12 +590,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -944,20 +951,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="8" max="8" width="18.36328125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -986,7 +993,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1010,7 +1017,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -1031,7 +1038,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -1052,7 +1059,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -1073,7 +1080,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1097,7 +1104,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -1117,6 +1124,16 @@
         <v>3</v>
       </c>
       <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F9" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>